<commit_message>
updated cpp files and data results
</commit_message>
<xml_diff>
--- a/test/test/benchmark_results.xlsx
+++ b/test/test/benchmark_results.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uri\csc411\test\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uri\csc411\Hyperthreading\test\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD97C4F-A6C2-4100-BB93-185757369247}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895A0DDF-2248-4533-ADA9-207DE92FE5AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{480B6FB2-1D4C-4C46-8A25-8B302E4C8EA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,20 +48,26 @@
     <t>duration(s)</t>
   </si>
   <si>
-    <t>Average Duration(s)</t>
+    <t>Average Duration(s) with hp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,7 +789,530 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t>Impact of Hyperthreading on 16 tasks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>No Hyperthreading</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]Sheet1!$G$2:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Threads</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sheet1!$I$2:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>16.005866666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2856133333333322</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3167033333333329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CFFA-466C-948D-FD8398B35743}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hyperthreading</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]Sheet1!$G$2:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 Threads</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4 Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sheet1!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15.659166666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7871966666666665</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1647633333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CFFA-466C-948D-FD8398B35743}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1338149024"/>
+        <c:axId val="1338151520"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1338149024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1338151520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1338151520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1300" baseline="0" dirty="0"/>
+                  <a:t>Duration (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1338149024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1368,6 +1901,502 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1406,7 +2435,92 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE2F8CD3-7969-400B-B9A3-F2906247B7FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="G2" t="str">
+            <v>1 Thread</v>
+          </cell>
+          <cell r="H2">
+            <v>15.659166666666666</v>
+          </cell>
+          <cell r="I2">
+            <v>16.005866666666666</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3" t="str">
+            <v>2 Threads</v>
+          </cell>
+          <cell r="H3">
+            <v>7.7871966666666665</v>
+          </cell>
+          <cell r="I3">
+            <v>8.2856133333333322</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4" t="str">
+            <v>4 Threads</v>
+          </cell>
+          <cell r="H4">
+            <v>4.1647633333333332</v>
+          </cell>
+          <cell r="I4">
+            <v>4.3167033333333329</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1706,16 +2820,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AA7D87-CB71-40DE-B908-0999B3D65C9B}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1794,7 +2908,7 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <f>AVERAGE(C3,D3,E3)</f>
+        <f t="shared" ref="J3:J49" si="0">AVERAGE(C3,D3,E3)</f>
         <v>2.0453899999999998</v>
       </c>
     </row>
@@ -1821,7 +2935,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <f>AVERAGE(C4,D4,E4)</f>
+        <f t="shared" si="0"/>
         <v>3.0061433333333336</v>
       </c>
     </row>
@@ -1848,7 +2962,7 @@
         <v>4</v>
       </c>
       <c r="J5">
-        <f>AVERAGE(C5,D5,E5)</f>
+        <f t="shared" si="0"/>
         <v>4.007343333333333</v>
       </c>
     </row>
@@ -1875,7 +2989,7 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <f>AVERAGE(C6,D6,E6)</f>
+        <f t="shared" si="0"/>
         <v>4.9934833333333337</v>
       </c>
     </row>
@@ -1902,7 +3016,7 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <f>AVERAGE(C7,D7,E7)</f>
+        <f t="shared" si="0"/>
         <v>6.0003166666666665</v>
       </c>
     </row>
@@ -1929,7 +3043,7 @@
         <v>7</v>
       </c>
       <c r="J8">
-        <f>AVERAGE(C8,D8,E8)</f>
+        <f t="shared" si="0"/>
         <v>7.0708333333333329</v>
       </c>
     </row>
@@ -1956,7 +3070,7 @@
         <v>8</v>
       </c>
       <c r="J9">
-        <f>AVERAGE(C9,D9,E9)</f>
+        <f t="shared" si="0"/>
         <v>8.0503266666666686</v>
       </c>
     </row>
@@ -1983,7 +3097,7 @@
         <v>9</v>
       </c>
       <c r="J10">
-        <f>AVERAGE(C10,D10,E10)</f>
+        <f t="shared" si="0"/>
         <v>9.027966666666666</v>
       </c>
     </row>
@@ -2010,7 +3124,7 @@
         <v>10</v>
       </c>
       <c r="J11">
-        <f>AVERAGE(C11,D11,E11)</f>
+        <f t="shared" si="0"/>
         <v>10.018146666666667</v>
       </c>
     </row>
@@ -2037,7 +3151,7 @@
         <v>11</v>
       </c>
       <c r="J12">
-        <f>AVERAGE(C12,D12,E12)</f>
+        <f t="shared" si="0"/>
         <v>11.015766666666666</v>
       </c>
     </row>
@@ -2064,7 +3178,7 @@
         <v>12</v>
       </c>
       <c r="J13">
-        <f>AVERAGE(C13,D13,E13)</f>
+        <f t="shared" si="0"/>
         <v>12.015766666666666</v>
       </c>
     </row>
@@ -2091,7 +3205,7 @@
         <v>13</v>
       </c>
       <c r="J14">
-        <f>AVERAGE(C14,D14,E14)</f>
+        <f t="shared" si="0"/>
         <v>13.020366666666668</v>
       </c>
     </row>
@@ -2118,7 +3232,7 @@
         <v>14</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(C15,D15,E15)</f>
+        <f t="shared" si="0"/>
         <v>14.012333333333332</v>
       </c>
     </row>
@@ -2145,7 +3259,7 @@
         <v>15</v>
       </c>
       <c r="J16">
-        <f>AVERAGE(C16,D16,E16)</f>
+        <f t="shared" si="0"/>
         <v>15.0655</v>
       </c>
     </row>
@@ -2172,7 +3286,7 @@
         <v>16</v>
       </c>
       <c r="J17">
-        <f>AVERAGE(C17,D17,E17)</f>
+        <f t="shared" si="0"/>
         <v>16.005866666666666</v>
       </c>
     </row>
@@ -2199,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <f>AVERAGE(C18,D18,E18)</f>
+        <f t="shared" si="0"/>
         <v>1.0023946666666665</v>
       </c>
     </row>
@@ -2226,7 +3340,7 @@
         <v>2</v>
       </c>
       <c r="J19">
-        <f>AVERAGE(C19,D19,E19)</f>
+        <f t="shared" si="0"/>
         <v>1.0313533333333333</v>
       </c>
     </row>
@@ -2253,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="J20">
-        <f>AVERAGE(C20,D20,E20)</f>
+        <f t="shared" si="0"/>
         <v>2.0184000000000002</v>
       </c>
     </row>
@@ -2280,7 +3394,7 @@
         <v>4</v>
       </c>
       <c r="J21">
-        <f>AVERAGE(C21,D21,E21)</f>
+        <f t="shared" si="0"/>
         <v>2.1065466666666666</v>
       </c>
     </row>
@@ -2307,7 +3421,7 @@
         <v>5</v>
       </c>
       <c r="J22">
-        <f>AVERAGE(C22,D22,E22)</f>
+        <f t="shared" si="0"/>
         <v>3.0757066666666666</v>
       </c>
     </row>
@@ -2334,7 +3448,7 @@
         <v>6</v>
       </c>
       <c r="J23">
-        <f>AVERAGE(C23,D23,E23)</f>
+        <f t="shared" si="0"/>
         <v>3.1669533333333333</v>
       </c>
     </row>
@@ -2361,7 +3475,7 @@
         <v>7</v>
       </c>
       <c r="J24">
-        <f>AVERAGE(C24,D24,E24)</f>
+        <f t="shared" si="0"/>
         <v>4.1857300000000004</v>
       </c>
     </row>
@@ -2388,7 +3502,7 @@
         <v>8</v>
       </c>
       <c r="J25">
-        <f>AVERAGE(C25,D25,E25)</f>
+        <f t="shared" si="0"/>
         <v>4.3822499999999991</v>
       </c>
     </row>
@@ -2415,7 +3529,7 @@
         <v>9</v>
       </c>
       <c r="J26">
-        <f>AVERAGE(C26,D26,E26)</f>
+        <f t="shared" si="0"/>
         <v>5.4249399999999994</v>
       </c>
     </row>
@@ -2442,7 +3556,7 @@
         <v>10</v>
       </c>
       <c r="J27">
-        <f>AVERAGE(C27,D27,E27)</f>
+        <f t="shared" si="0"/>
         <v>5.2585033333333335</v>
       </c>
     </row>
@@ -2469,7 +3583,7 @@
         <v>11</v>
       </c>
       <c r="J28">
-        <f>AVERAGE(C28,D28,E28)</f>
+        <f t="shared" si="0"/>
         <v>6.2035666666666671</v>
       </c>
     </row>
@@ -2496,7 +3610,7 @@
         <v>12</v>
       </c>
       <c r="J29">
-        <f>AVERAGE(C29,D29,E29)</f>
+        <f t="shared" si="0"/>
         <v>6.2024866666666663</v>
       </c>
     </row>
@@ -2523,7 +3637,7 @@
         <v>13</v>
       </c>
       <c r="J30">
-        <f>AVERAGE(C30,D30,E30)</f>
+        <f t="shared" si="0"/>
         <v>7.2359666666666662</v>
       </c>
     </row>
@@ -2550,7 +3664,7 @@
         <v>14</v>
       </c>
       <c r="J31">
-        <f>AVERAGE(C31,D31,E31)</f>
+        <f t="shared" si="0"/>
         <v>7.2563699999999995</v>
       </c>
     </row>
@@ -2577,11 +3691,11 @@
         <v>15</v>
       </c>
       <c r="J32">
-        <f>AVERAGE(C32,D32,E32)</f>
+        <f t="shared" si="0"/>
         <v>8.2447333333333344</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2604,11 +3718,11 @@
         <v>16</v>
       </c>
       <c r="J33">
-        <f>AVERAGE(C33,D33,E33)</f>
+        <f t="shared" si="0"/>
         <v>8.2856133333333322</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2631,11 +3745,11 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <f>AVERAGE(C34,D34,E34)</f>
+        <f t="shared" si="0"/>
         <v>1.016637</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2658,11 +3772,11 @@
         <v>2</v>
       </c>
       <c r="J35">
-        <f>AVERAGE(C35,D35,E35)</f>
+        <f t="shared" si="0"/>
         <v>1.0360466666666668</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2685,11 +3799,12 @@
         <v>3</v>
       </c>
       <c r="J36">
-        <f>AVERAGE(C36,D36,E36)</f>
+        <f t="shared" si="0"/>
         <v>1.0580799999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2712,11 +3827,11 @@
         <v>4</v>
       </c>
       <c r="J37">
-        <f>AVERAGE(C37,D37,E37)</f>
+        <f t="shared" si="0"/>
         <v>1.1064800000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2739,11 +3854,11 @@
         <v>5</v>
       </c>
       <c r="J38">
-        <f>AVERAGE(C38,D38,E38)</f>
+        <f t="shared" si="0"/>
         <v>2.0689533333333334</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2766,11 +3881,11 @@
         <v>6</v>
       </c>
       <c r="J39">
-        <f>AVERAGE(C39,D39,E39)</f>
+        <f t="shared" si="0"/>
         <v>2.0963766666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2793,11 +3908,11 @@
         <v>7</v>
       </c>
       <c r="J40">
-        <f>AVERAGE(C40,D40,E40)</f>
+        <f t="shared" si="0"/>
         <v>2.1443800000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2820,11 +3935,11 @@
         <v>8</v>
       </c>
       <c r="J41">
-        <f>AVERAGE(C41,D41,E41)</f>
+        <f t="shared" si="0"/>
         <v>2.1408999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2847,11 +3962,11 @@
         <v>9</v>
       </c>
       <c r="J42">
-        <f>AVERAGE(C42,D42,E42)</f>
+        <f t="shared" si="0"/>
         <v>3.1278533333333338</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2874,11 +3989,11 @@
         <v>10</v>
       </c>
       <c r="J43">
-        <f>AVERAGE(C43,D43,E43)</f>
+        <f t="shared" si="0"/>
         <v>3.1782599999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2901,11 +4016,11 @@
         <v>11</v>
       </c>
       <c r="J44">
-        <f>AVERAGE(C44,D44,E44)</f>
+        <f t="shared" si="0"/>
         <v>3.1910533333333331</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2928,11 +4043,11 @@
         <v>12</v>
       </c>
       <c r="J45">
-        <f>AVERAGE(C45,D45,E45)</f>
+        <f t="shared" si="0"/>
         <v>3.2454533333333333</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -2955,11 +4070,11 @@
         <v>13</v>
       </c>
       <c r="J46">
-        <f>AVERAGE(C46,D46,E46)</f>
+        <f t="shared" si="0"/>
         <v>4.277236666666667</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2982,11 +4097,11 @@
         <v>14</v>
       </c>
       <c r="J47">
-        <f>AVERAGE(C47,D47,E47)</f>
+        <f t="shared" si="0"/>
         <v>4.2720799999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4</v>
       </c>
@@ -3009,7 +4124,7 @@
         <v>15</v>
       </c>
       <c r="J48">
-        <f>AVERAGE(C48,D48,E48)</f>
+        <f t="shared" si="0"/>
         <v>4.3048699999999993</v>
       </c>
     </row>
@@ -3036,7 +4151,7 @@
         <v>16</v>
       </c>
       <c r="J49">
-        <f>AVERAGE(C49,D49,E49)</f>
+        <f t="shared" si="0"/>
         <v>4.3167033333333329</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final code with thread pool
</commit_message>
<xml_diff>
--- a/test/test/benchmark_results.xlsx
+++ b/test/test/benchmark_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uri\csc411\Hyperthreading\test\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895A0DDF-2248-4533-ADA9-207DE92FE5AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E76A0E-F176-437C-843A-5FD6B05881E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{480B6FB2-1D4C-4C46-8A25-8B302E4C8EA2}"/>
   </bookViews>
@@ -923,7 +923,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$I$2:$I$4</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>16.005866666666666</c:v>
@@ -988,7 +988,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$H$2:$H$4</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>15.659166666666666</c:v>
@@ -1145,7 +1145,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2437,16 +2437,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2822,8 +2822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AA7D87-CB71-40DE-B908-0999B3D65C9B}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>